<commit_message>
Updating emergency and elective column
</commit_message>
<xml_diff>
--- a/Copy of Mitigator list.xlsx
+++ b/Copy of Mitigator list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/sarah_lucas3_nhs_net/Documents/Documents/2025 projects/Describing NHP mitigators/nhp_community_mitigators/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="95" documentId="8_{1C736938-C755-48C2-B0DB-C2941D05B2C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80C7949E-5368-40FF-815A-EF559B80E45B}"/>
+  <xr:revisionPtr revIDLastSave="124" documentId="8_{1C736938-C755-48C2-B0DB-C2941D05B2C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24E356A1-414D-4E2A-983F-4EA7537B12E8}"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="0" windowWidth="20928" windowHeight="13800" xr2:uid="{C8819F7C-E552-47C7-93CD-68F88BD9D686}"/>
+    <workbookView xWindow="120" yWindow="1344" windowWidth="20928" windowHeight="13800" xr2:uid="{C8819F7C-E552-47C7-93CD-68F88BD9D686}"/>
   </bookViews>
   <sheets>
     <sheet name="List of all AMs" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="292">
   <si>
     <t>Mitigator code</t>
   </si>
@@ -912,17 +912,14 @@
     <t>Only need to be entered in the data frame once</t>
   </si>
   <si>
-    <t>emergency</t>
-  </si>
-  <si>
-    <t>elective</t>
+    <t>Checked emergency vs elective against new python code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1060,7 +1057,12 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1499,20 +1501,38 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1889,10 +1909,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{212D035E-5B85-4011-9BFC-B0BBE05A06BD}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:K93"/>
+  <dimension ref="A1:I93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="E19" workbookViewId="0">
+      <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1904,10 +1924,9 @@
     <col min="5" max="5" width="65.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.44140625" customWidth="1"/>
-    <col min="9" max="9" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1932,14 +1951,8 @@
       <c r="H1" t="s">
         <v>289</v>
       </c>
-      <c r="I1" t="s">
-        <v>291</v>
-      </c>
-      <c r="J1" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1956,7 +1969,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1973,7 +1986,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1990,7 +2003,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -2007,7 +2020,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2024,7 +2037,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -2041,7 +2054,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -2058,7 +2071,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -2075,7 +2088,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -2092,7 +2105,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -2109,7 +2122,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -2126,7 +2139,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -2143,7 +2156,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -2160,7 +2173,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -2177,7 +2190,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -2194,7 +2207,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -2211,118 +2224,114 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>55</v>
       </c>
       <c r="B18" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="5" t="s">
+      <c r="C18" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="19" t="s">
         <v>286</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="19">
         <v>1</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="20">
         <v>1</v>
       </c>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="1"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I18" s="9" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>59</v>
       </c>
       <c r="B19" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="C19" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="9">
         <v>1</v>
       </c>
-      <c r="H19" s="8">
+      <c r="H19" s="22">
         <v>1</v>
       </c>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-    </row>
-    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>62</v>
       </c>
       <c r="B20" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="10" t="s">
+      <c r="C20" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="24" t="s">
         <v>286</v>
       </c>
-      <c r="G20" s="10">
+      <c r="G20" s="24">
         <v>1</v>
       </c>
-      <c r="H20" s="11">
+      <c r="H20" s="25">
         <v>1</v>
       </c>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>65</v>
       </c>
       <c r="B21" t="s">
         <v>56</v>
       </c>
-      <c r="C21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="C21" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="15" t="s">
         <v>286</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="15">
         <v>1</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>68</v>
       </c>
@@ -2348,33 +2357,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>71</v>
       </c>
       <c r="B23" t="s">
         <v>56</v>
       </c>
-      <c r="C23" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="C23" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="15" t="s">
         <v>286</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="15">
         <v>1</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>74</v>
       </c>
@@ -2391,63 +2400,59 @@
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>77</v>
       </c>
       <c r="B25" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="5" t="s">
+      <c r="C25" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E25" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="27" t="s">
         <v>286</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G25" s="19">
         <v>1</v>
       </c>
-      <c r="H25" s="6">
+      <c r="H25" s="20">
         <v>1</v>
       </c>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-    </row>
-    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>80</v>
       </c>
       <c r="B26" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="10" t="s">
+      <c r="C26" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="F26" s="29" t="s">
         <v>286</v>
       </c>
-      <c r="G26" s="10">
+      <c r="G26" s="24">
         <v>1</v>
       </c>
-      <c r="H26" s="11">
+      <c r="H26" s="25">
         <v>1</v>
       </c>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-    </row>
-    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>83</v>
       </c>
@@ -2464,7 +2469,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>86</v>
       </c>
@@ -2481,7 +2486,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>89</v>
       </c>
@@ -2498,7 +2503,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>92</v>
       </c>
@@ -2515,7 +2520,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>95</v>
       </c>
@@ -2532,7 +2537,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>98</v>
       </c>
@@ -2549,89 +2554,85 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>101</v>
       </c>
       <c r="B33" t="s">
         <v>56</v>
       </c>
-      <c r="C33" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="C33" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="15" t="s">
         <v>286</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="16">
         <v>1</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>104</v>
       </c>
       <c r="B34" t="s">
         <v>56</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34" s="5" t="s">
+      <c r="C34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="E34" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="F34" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="G34" s="5">
+      <c r="G34" s="10">
         <v>1</v>
       </c>
-      <c r="H34" s="6">
+      <c r="H34" s="11">
         <v>0</v>
       </c>
-      <c r="I34" s="12"/>
-      <c r="J34" s="12"/>
-    </row>
-    <row r="35" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>107</v>
       </c>
       <c r="B35" t="s">
         <v>56</v>
       </c>
-      <c r="C35" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" s="10" t="s">
+      <c r="C35" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E35" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="F35" s="10" t="s">
+      <c r="F35" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="G35" s="10">
+      <c r="G35" s="12">
         <v>1</v>
       </c>
-      <c r="H35" s="11">
+      <c r="H35" s="13">
         <v>0</v>
       </c>
-      <c r="I35" s="12"/>
-      <c r="J35" s="12"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>110</v>
       </c>
@@ -2650,14 +2651,14 @@
       <c r="F36" t="s">
         <v>286</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="14">
         <v>1</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>113</v>
       </c>
@@ -2676,14 +2677,14 @@
       <c r="F37" t="s">
         <v>286</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="14">
         <v>1</v>
       </c>
-      <c r="H37">
+      <c r="H37" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>116</v>
       </c>
@@ -2702,14 +2703,14 @@
       <c r="F38" t="s">
         <v>286</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="14">
         <v>1</v>
       </c>
-      <c r="H38">
+      <c r="H38" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>119</v>
       </c>
@@ -2728,14 +2729,14 @@
       <c r="F39" t="s">
         <v>286</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="14">
         <v>1</v>
       </c>
-      <c r="H39">
+      <c r="H39" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>122</v>
       </c>
@@ -2754,14 +2755,14 @@
       <c r="F40" t="s">
         <v>286</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="14">
         <v>1</v>
       </c>
-      <c r="H40">
+      <c r="H40" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>125</v>
       </c>
@@ -2780,14 +2781,14 @@
       <c r="F41" t="s">
         <v>286</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="14">
         <v>1</v>
       </c>
-      <c r="H41">
+      <c r="H41" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>128</v>
       </c>
@@ -2806,40 +2807,40 @@
       <c r="F42" t="s">
         <v>286</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="14">
         <v>1</v>
       </c>
-      <c r="H42">
+      <c r="H42" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>131</v>
       </c>
       <c r="B43" t="s">
         <v>56</v>
       </c>
-      <c r="C43" t="s">
-        <v>7</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="C43" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" s="30" t="s">
         <v>286</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="9">
         <v>1</v>
       </c>
-      <c r="H43">
+      <c r="H43" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>134</v>
       </c>
@@ -2858,14 +2859,14 @@
       <c r="F44" t="s">
         <v>286</v>
       </c>
-      <c r="G44">
+      <c r="G44" s="7">
         <v>1</v>
       </c>
-      <c r="H44">
+      <c r="H44" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>137</v>
       </c>
@@ -2884,94 +2885,90 @@
       <c r="F45" t="s">
         <v>286</v>
       </c>
-      <c r="G45">
+      <c r="G45" s="7">
         <v>1</v>
       </c>
-      <c r="H45">
+      <c r="H45" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>140</v>
       </c>
       <c r="B46" t="s">
         <v>56</v>
       </c>
-      <c r="C46" t="s">
-        <v>7</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="C46" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F46" s="15" t="s">
         <v>286</v>
       </c>
-      <c r="G46">
+      <c r="G46" s="17">
         <v>1</v>
       </c>
-      <c r="H46">
+      <c r="H46" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>143</v>
       </c>
       <c r="B47" t="s">
         <v>56</v>
       </c>
-      <c r="C47" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D47" s="2" t="s">
+      <c r="C47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="E47" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="F47" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="G47" s="2">
+      <c r="G47" s="8">
         <v>1</v>
       </c>
-      <c r="H47" s="2">
+      <c r="H47" s="8">
         <v>0</v>
       </c>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>146</v>
       </c>
       <c r="B48" t="s">
         <v>56</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D48" s="2" t="s">
+      <c r="C48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="E48" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="F48" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="G48" s="2">
+      <c r="G48" s="8">
         <v>1</v>
       </c>
-      <c r="H48" s="2">
+      <c r="H48" s="8">
         <v>0</v>
       </c>
-      <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
@@ -2992,10 +2989,10 @@
       <c r="F49" t="s">
         <v>286</v>
       </c>
-      <c r="G49">
+      <c r="G49" s="7">
         <v>1</v>
       </c>
-      <c r="H49">
+      <c r="H49" s="7">
         <v>0</v>
       </c>
     </row>
@@ -3018,10 +3015,10 @@
       <c r="F50" t="s">
         <v>286</v>
       </c>
-      <c r="G50">
+      <c r="G50" s="7">
         <v>1</v>
       </c>
-      <c r="H50">
+      <c r="H50" s="7">
         <v>0</v>
       </c>
     </row>
@@ -3180,10 +3177,10 @@
       <c r="F59" t="s">
         <v>286</v>
       </c>
-      <c r="G59">
+      <c r="G59" s="7">
         <v>1</v>
       </c>
-      <c r="H59">
+      <c r="H59" s="7">
         <v>0</v>
       </c>
     </row>
@@ -3272,7 +3269,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>198</v>
       </c>
@@ -3289,7 +3286,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>201</v>
       </c>
@@ -3306,7 +3303,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>204</v>
       </c>
@@ -3323,7 +3320,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>207</v>
       </c>
@@ -3340,7 +3337,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>210</v>
       </c>
@@ -3357,7 +3354,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>213</v>
       </c>
@@ -3374,7 +3371,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>216</v>
       </c>
@@ -3391,7 +3388,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>219</v>
       </c>
@@ -3408,7 +3405,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>222</v>
       </c>
@@ -3425,7 +3422,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>225</v>
       </c>
@@ -3444,14 +3441,14 @@
       <c r="F74" t="s">
         <v>286</v>
       </c>
-      <c r="G74">
+      <c r="G74" s="7">
         <v>1</v>
       </c>
-      <c r="H74">
+      <c r="H74" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>228</v>
       </c>
@@ -3470,73 +3467,69 @@
       <c r="F75" t="s">
         <v>286</v>
       </c>
-      <c r="G75">
+      <c r="G75" s="7">
         <v>1</v>
       </c>
-      <c r="H75">
+      <c r="H75" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>231</v>
       </c>
       <c r="B76" t="s">
         <v>56</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C76" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="D76" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="E76" s="2" t="s">
+      <c r="E76" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="F76" s="2" t="s">
+      <c r="F76" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="G76" s="2">
+      <c r="G76" s="8">
         <v>1</v>
       </c>
-      <c r="H76" s="2">
+      <c r="H76" s="8">
         <v>0</v>
       </c>
-      <c r="I76" s="2"/>
-      <c r="J76" s="2"/>
-      <c r="K76" s="3" t="s">
+      <c r="I76" s="2" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>234</v>
       </c>
       <c r="B77" t="s">
         <v>56</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="C77" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D77" s="2" t="s">
+      <c r="D77" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="E77" s="2" t="s">
+      <c r="E77" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="F77" s="2" t="s">
+      <c r="F77" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="G77" s="2">
+      <c r="G77" s="8">
         <v>1</v>
       </c>
-      <c r="H77" s="2">
+      <c r="H77" s="8">
         <v>0</v>
       </c>
-      <c r="I77" s="2"/>
-      <c r="J77" s="2"/>
-    </row>
-    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>237</v>
       </c>
@@ -3553,7 +3546,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>241</v>
       </c>
@@ -3570,7 +3563,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>244</v>
       </c>
@@ -3817,6 +3810,7 @@
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
updating elective and emergency columns
</commit_message>
<xml_diff>
--- a/Copy of Mitigator list.xlsx
+++ b/Copy of Mitigator list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/sarah_lucas3_nhs_net/Documents/Documents/2025 projects/Describing NHP mitigators/nhp_community_mitigators/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="124" documentId="8_{1C736938-C755-48C2-B0DB-C2941D05B2C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24E356A1-414D-4E2A-983F-4EA7537B12E8}"/>
+  <xr:revisionPtr revIDLastSave="134" documentId="8_{1C736938-C755-48C2-B0DB-C2941D05B2C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDE6F3E3-AB70-4C03-B3E5-A39AE872DE62}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="1344" windowWidth="20928" windowHeight="13800" xr2:uid="{C8819F7C-E552-47C7-93CD-68F88BD9D686}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{C8819F7C-E552-47C7-93CD-68F88BD9D686}"/>
   </bookViews>
   <sheets>
     <sheet name="List of all AMs" sheetId="1" r:id="rId1"/>
@@ -1501,7 +1501,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -1509,17 +1509,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1533,6 +1528,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1911,8 +1907,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E19" workbookViewId="0">
-      <selection activeCell="L43" sqref="L43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2231,25 +2227,25 @@
       <c r="B18" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="19" t="s">
+      <c r="C18" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="E18" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="19" t="s">
+      <c r="F18" s="14" t="s">
         <v>286</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G18" s="14">
         <v>1</v>
       </c>
-      <c r="H18" s="20">
+      <c r="H18" s="15">
         <v>1</v>
       </c>
-      <c r="I18" s="9" t="s">
+      <c r="I18" s="7" t="s">
         <v>291</v>
       </c>
     </row>
@@ -2260,22 +2256,22 @@
       <c r="B19" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="9" t="s">
+      <c r="C19" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="7">
         <v>1</v>
       </c>
-      <c r="H19" s="22">
+      <c r="H19" s="17">
         <v>1</v>
       </c>
     </row>
@@ -2286,22 +2282,22 @@
       <c r="B20" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="24" t="s">
+      <c r="C20" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="E20" s="24" t="s">
+      <c r="E20" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="F20" s="24" t="s">
+      <c r="F20" s="19" t="s">
         <v>286</v>
       </c>
-      <c r="G20" s="24">
+      <c r="G20" s="19">
         <v>1</v>
       </c>
-      <c r="H20" s="25">
+      <c r="H20" s="20">
         <v>1</v>
       </c>
     </row>
@@ -2312,22 +2308,22 @@
       <c r="B21" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="15" t="s">
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" t="s">
         <v>66</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" t="s">
         <v>67</v>
       </c>
-      <c r="F21" s="15" t="s">
+      <c r="F21" t="s">
         <v>286</v>
       </c>
-      <c r="G21" s="15">
+      <c r="G21">
         <v>1</v>
       </c>
-      <c r="H21" s="15">
+      <c r="H21">
         <v>0</v>
       </c>
     </row>
@@ -2364,22 +2360,22 @@
       <c r="B23" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="15" t="s">
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
         <v>72</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E23" t="s">
         <v>73</v>
       </c>
-      <c r="F23" s="15" t="s">
+      <c r="F23" t="s">
         <v>286</v>
       </c>
-      <c r="G23" s="15">
+      <c r="G23">
         <v>1</v>
       </c>
-      <c r="H23" s="15">
+      <c r="H23">
         <v>0</v>
       </c>
     </row>
@@ -2407,22 +2403,22 @@
       <c r="B25" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="27" t="s">
+      <c r="C25" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="E25" s="27" t="s">
+      <c r="E25" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="F25" s="27" t="s">
+      <c r="F25" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="G25" s="19">
+      <c r="G25" s="14">
         <v>1</v>
       </c>
-      <c r="H25" s="20">
+      <c r="H25" s="15">
         <v>1</v>
       </c>
     </row>
@@ -2433,22 +2429,22 @@
       <c r="B26" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="29" t="s">
+      <c r="C26" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="E26" s="29" t="s">
+      <c r="E26" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="F26" s="29" t="s">
+      <c r="F26" s="24" t="s">
         <v>286</v>
       </c>
-      <c r="G26" s="24">
+      <c r="G26" s="19">
         <v>1</v>
       </c>
-      <c r="H26" s="25">
+      <c r="H26" s="20">
         <v>1</v>
       </c>
     </row>
@@ -2561,22 +2557,22 @@
       <c r="B33" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" s="15" t="s">
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" t="s">
         <v>102</v>
       </c>
-      <c r="E33" s="15" t="s">
+      <c r="E33" t="s">
         <v>103</v>
       </c>
-      <c r="F33" s="15" t="s">
+      <c r="F33" t="s">
         <v>286</v>
       </c>
-      <c r="G33" s="16">
+      <c r="G33" s="12">
         <v>1</v>
       </c>
-      <c r="H33" s="16">
+      <c r="H33" s="12">
         <v>0</v>
       </c>
     </row>
@@ -2599,10 +2595,10 @@
       <c r="F34" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="G34" s="10">
+      <c r="G34" s="8">
         <v>1</v>
       </c>
-      <c r="H34" s="11">
+      <c r="H34" s="9">
         <v>0</v>
       </c>
     </row>
@@ -2625,10 +2621,10 @@
       <c r="F35" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="G35" s="12">
+      <c r="G35" s="10">
         <v>1</v>
       </c>
-      <c r="H35" s="13">
+      <c r="H35" s="11">
         <v>0</v>
       </c>
     </row>
@@ -2651,10 +2647,10 @@
       <c r="F36" t="s">
         <v>286</v>
       </c>
-      <c r="G36" s="14">
+      <c r="G36" s="12">
         <v>1</v>
       </c>
-      <c r="H36" s="14">
+      <c r="H36" s="12">
         <v>0</v>
       </c>
     </row>
@@ -2677,10 +2673,10 @@
       <c r="F37" t="s">
         <v>286</v>
       </c>
-      <c r="G37" s="14">
+      <c r="G37" s="12">
         <v>1</v>
       </c>
-      <c r="H37" s="14">
+      <c r="H37" s="12">
         <v>0</v>
       </c>
     </row>
@@ -2703,10 +2699,10 @@
       <c r="F38" t="s">
         <v>286</v>
       </c>
-      <c r="G38" s="14">
+      <c r="G38" s="12">
         <v>1</v>
       </c>
-      <c r="H38" s="14">
+      <c r="H38" s="12">
         <v>0</v>
       </c>
     </row>
@@ -2729,10 +2725,10 @@
       <c r="F39" t="s">
         <v>286</v>
       </c>
-      <c r="G39" s="14">
+      <c r="G39" s="12">
         <v>1</v>
       </c>
-      <c r="H39" s="14">
+      <c r="H39" s="12">
         <v>0</v>
       </c>
     </row>
@@ -2755,10 +2751,10 @@
       <c r="F40" t="s">
         <v>286</v>
       </c>
-      <c r="G40" s="14">
+      <c r="G40" s="12">
         <v>1</v>
       </c>
-      <c r="H40" s="14">
+      <c r="H40" s="12">
         <v>0</v>
       </c>
     </row>
@@ -2781,10 +2777,10 @@
       <c r="F41" t="s">
         <v>286</v>
       </c>
-      <c r="G41" s="14">
+      <c r="G41" s="12">
         <v>1</v>
       </c>
-      <c r="H41" s="14">
+      <c r="H41" s="12">
         <v>0</v>
       </c>
     </row>
@@ -2807,10 +2803,10 @@
       <c r="F42" t="s">
         <v>286</v>
       </c>
-      <c r="G42" s="14">
+      <c r="G42" s="12">
         <v>1</v>
       </c>
-      <c r="H42" s="14">
+      <c r="H42" s="12">
         <v>0</v>
       </c>
     </row>
@@ -2821,22 +2817,22 @@
       <c r="B43" t="s">
         <v>56</v>
       </c>
-      <c r="C43" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D43" s="30" t="s">
+      <c r="C43" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="E43" s="30" t="s">
+      <c r="E43" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="F43" s="30" t="s">
+      <c r="F43" s="25" t="s">
         <v>286</v>
       </c>
-      <c r="G43" s="9">
+      <c r="G43" s="7">
         <v>1</v>
       </c>
-      <c r="H43" s="9">
+      <c r="H43" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2859,10 +2855,10 @@
       <c r="F44" t="s">
         <v>286</v>
       </c>
-      <c r="G44" s="7">
+      <c r="G44" s="12">
         <v>1</v>
       </c>
-      <c r="H44" s="7">
+      <c r="H44" s="12">
         <v>0</v>
       </c>
     </row>
@@ -2885,10 +2881,10 @@
       <c r="F45" t="s">
         <v>286</v>
       </c>
-      <c r="G45" s="7">
+      <c r="G45" s="12">
         <v>1</v>
       </c>
-      <c r="H45" s="7">
+      <c r="H45" s="12">
         <v>0</v>
       </c>
     </row>
@@ -2899,22 +2895,22 @@
       <c r="B46" t="s">
         <v>56</v>
       </c>
-      <c r="C46" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D46" s="15" t="s">
+      <c r="C46" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="E46" s="15" t="s">
+      <c r="E46" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="F46" s="15" t="s">
+      <c r="F46" s="25" t="s">
         <v>286</v>
       </c>
-      <c r="G46" s="17">
+      <c r="G46" s="7">
         <v>1</v>
       </c>
-      <c r="H46" s="17">
+      <c r="H46" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2937,10 +2933,10 @@
       <c r="F47" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="G47" s="8">
+      <c r="G47" s="26">
         <v>1</v>
       </c>
-      <c r="H47" s="8">
+      <c r="H47" s="26">
         <v>0</v>
       </c>
     </row>
@@ -2963,10 +2959,10 @@
       <c r="F48" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="G48" s="8">
+      <c r="G48" s="26">
         <v>1</v>
       </c>
-      <c r="H48" s="8">
+      <c r="H48" s="26">
         <v>0</v>
       </c>
     </row>
@@ -2989,10 +2985,10 @@
       <c r="F49" t="s">
         <v>286</v>
       </c>
-      <c r="G49" s="7">
+      <c r="G49" s="12">
         <v>1</v>
       </c>
-      <c r="H49" s="7">
+      <c r="H49" s="12">
         <v>0</v>
       </c>
     </row>
@@ -3015,10 +3011,10 @@
       <c r="F50" t="s">
         <v>286</v>
       </c>
-      <c r="G50" s="7">
+      <c r="G50" s="12">
         <v>1</v>
       </c>
-      <c r="H50" s="7">
+      <c r="H50" s="12">
         <v>0</v>
       </c>
     </row>
@@ -3177,10 +3173,10 @@
       <c r="F59" t="s">
         <v>286</v>
       </c>
-      <c r="G59" s="7">
+      <c r="G59" s="12">
         <v>1</v>
       </c>
-      <c r="H59" s="7">
+      <c r="H59" s="12">
         <v>0</v>
       </c>
     </row>
@@ -3441,10 +3437,10 @@
       <c r="F74" t="s">
         <v>286</v>
       </c>
-      <c r="G74" s="7">
+      <c r="G74" s="12">
         <v>1</v>
       </c>
-      <c r="H74" s="7">
+      <c r="H74" s="12">
         <v>0</v>
       </c>
     </row>
@@ -3467,10 +3463,10 @@
       <c r="F75" t="s">
         <v>286</v>
       </c>
-      <c r="G75" s="7">
+      <c r="G75" s="12">
         <v>1</v>
       </c>
-      <c r="H75" s="7">
+      <c r="H75" s="12">
         <v>0</v>
       </c>
     </row>
@@ -3493,10 +3489,10 @@
       <c r="F76" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="G76" s="8">
+      <c r="G76" s="26">
         <v>1</v>
       </c>
-      <c r="H76" s="8">
+      <c r="H76" s="26">
         <v>0</v>
       </c>
       <c r="I76" s="2" t="s">
@@ -3522,10 +3518,10 @@
       <c r="F77" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="G77" s="8">
+      <c r="G77" s="26">
         <v>1</v>
       </c>
-      <c r="H77" s="8">
+      <c r="H77" s="26">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding summary of total mitigation page template
</commit_message>
<xml_diff>
--- a/Copy of Mitigator list.xlsx
+++ b/Copy of Mitigator list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/sarah_lucas3_nhs_net/Documents/Documents/2025 projects/Describing NHP mitigators/nhp_community_mitigators/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="134" documentId="8_{1C736938-C755-48C2-B0DB-C2941D05B2C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDE6F3E3-AB70-4C03-B3E5-A39AE872DE62}"/>
+  <xr:revisionPtr revIDLastSave="135" documentId="8_{1C736938-C755-48C2-B0DB-C2941D05B2C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42B93D48-2320-4D5A-A512-532DF2B615A3}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{C8819F7C-E552-47C7-93CD-68F88BD9D686}"/>
   </bookViews>
@@ -1907,15 +1907,15 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18:E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5546875" customWidth="1"/>
     <col min="4" max="4" width="49" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="65.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>

</xml_diff>